<commit_message>
moving on with the assignment
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Bubu\St Martins\Degree Year 2\SMc20374 programming for prototyping\python_section_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489EA23E-D86F-45DB-9553-62D84925AE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F4A302-E92D-4A2B-8A40-AA37282D8AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,12 @@
     <sheet name="base_w_plikHM_TTTEEE_lowl_lowE_" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t xml:space="preserve"> omegabh2</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>ns[6]</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -759,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -772,7 +778,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -784,39 +790,40 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -873,6 +880,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>360217</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>135083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>439350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>54871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3295DEEA-8480-81AC-E907-5D5F4EF43913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5011881" y="318656"/>
+          <a:ext cx="3639058" cy="1028844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3729,19 +3785,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586EC82B-77CE-4FA5-B7DA-44E778EA6646}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="9.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
@@ -3752,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -3762,8 +3822,17 @@
       <c r="C2" s="10">
         <v>-8.5427476999999998E-8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -3773,8 +3842,27 @@
       <c r="C3" s="10">
         <v>1.3503565999999999E-6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" s="21">
+        <f>(B2+C3)/2</f>
+        <v>6.8528594699999998E-7</v>
+      </c>
+      <c r="F3" s="21">
+        <f>(B2+C3)/2</f>
+        <v>6.8528594699999998E-7</v>
+      </c>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="21">
+        <f>((B2-C3)*(B2-C3))/4</f>
+        <v>4.4231897348184634E-13</v>
+      </c>
+      <c r="F4" s="21">
+        <f>((B2-C3)*(B2-C3))/4</f>
+        <v>4.4231897348184634E-13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>26</v>
       </c>
@@ -3784,8 +3872,16 @@
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" s="21">
+        <f>E4+(B3*B3)</f>
+        <v>4.4961682730843187E-13</v>
+      </c>
+      <c r="F5" s="21">
+        <f>F4+(B3*B3)</f>
+        <v>4.4961682730843187E-13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -3795,8 +3891,16 @@
       <c r="C6" s="10">
         <v>-2.0987421999999998E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <f>SQRT(E5)</f>
+        <v>6.7053473236546959E-7</v>
+      </c>
+      <c r="F6">
+        <f>SQRT(F5)</f>
+        <v>6.7053473236546959E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
@@ -3806,8 +3910,26 @@
       <c r="C7" s="10">
         <v>9.4181001000000002E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" s="21">
+        <f>E3+E6</f>
+        <v>1.3558206793654697E-6</v>
+      </c>
+      <c r="F7" s="21">
+        <f>F3-F6</f>
+        <v>1.4751214634530386E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="2">
+        <f>SQRT(E7)</f>
+        <v>1.1643971312939026E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <f>SQRT(F7)</f>
+        <v>1.2145457848319423E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
@@ -3817,8 +3939,16 @@
       <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <f>E8*1.52</f>
+        <v>1.7698836395667319E-3</v>
+      </c>
+      <c r="F9">
+        <f>F8*1.52</f>
+        <v>1.8461095929445524E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
@@ -3829,7 +3959,7 @@
         <v>5.9627878999999996E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
@@ -3839,8 +3969,12 @@
       <c r="C11" s="10">
         <v>1.6375672999999999E-5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11" s="21">
+        <f>(2*B3)/(B2-C3)</f>
+        <v>0.12844872437936306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
@@ -3851,7 +3985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>2</v>
       </c>
@@ -3862,7 +3996,7 @@
         <v>3.2934842999999999E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>3</v>
       </c>
@@ -3871,10 +4005,25 @@
       </c>
       <c r="C15" s="6">
         <v>9.4181001000000002E-4</v>
+      </c>
+      <c r="E15" s="10">
+        <v>2.0215294E-8</v>
+      </c>
+      <c r="F15" s="10">
+        <v>-8.5427476999999998E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="10">
+        <v>-8.5427476999999998E-8</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1.3503565999999999E-6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>